<commit_message>
student details issues resolve
</commit_message>
<xml_diff>
--- a/TestDataFile/Login.xlsx
+++ b/TestDataFile/Login.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amity.DESKTOP-HKLU73H\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amity.DESKTOP-HKLU73H\git\selenium-studentportal\TestDataFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>UserName</t>
   </si>
@@ -32,10 +32,7 @@
     <t>Password</t>
   </si>
   <si>
-    <t>ngasce@775</t>
-  </si>
-  <si>
-    <t>grhru</t>
+    <t>Ngasce@123</t>
   </si>
 </sst>
 </file>
@@ -98,16 +95,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -389,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,14 +411,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>54443434</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
get assignment from ui
</commit_message>
<xml_diff>
--- a/TestDataFile/Login.xlsx
+++ b/TestDataFile/Login.xlsx
@@ -32,7 +32,7 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Jitu@1990</t>
+    <t>Sonu@261295</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +410,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>77118915395</v>
+        <v>77119564838</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Add Acad year and month
</commit_message>
<xml_diff>
--- a/TestDataFile/Login.xlsx
+++ b/TestDataFile/Login.xlsx
@@ -32,7 +32,7 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Sonu@261295</t>
+    <t>Password@123</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +410,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>77119564838</v>
+        <v>77118576036</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
code clean in student Basic info
</commit_message>
<xml_diff>
--- a/TestDataFile/Login.xlsx
+++ b/TestDataFile/Login.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amity.DESKTOP-HKLU73H\git\selenium-studentportal\TestDataFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amit.yadav.ext\git\selenium-studentportal\TestDataFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB864B1C-C3A8-4EE8-B60B-9864661C8627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login_credentials" sheetId="1" r:id="rId1"/>
@@ -32,25 +33,17 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Password@123</t>
+    <t>Darshu@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -94,22 +87,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -387,11 +374,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,19 +396,15 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>77118576036</v>
+      <c r="A2">
+        <v>77122558691</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="Jitu@1990"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>